<commit_message>
final save for embedded dev 26
</commit_message>
<xml_diff>
--- a/boards/embedded-dev-26/JLC_Order/BOM.xlsx
+++ b/boards/embedded-dev-26/JLC_Order/BOM.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amsie\OneDrive\Documents\GitHub\mrover-electrical\boards\embedded-dev-26\Project Outputs for embedded-dev-26\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amsie\OneDrive\Documents\GitHub\mrover-electrical\boards\embedded-dev-26\JLC_Order\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22F7E651-9F14-4674-8524-87180F877228}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF3A936-3EC7-46A9-A619-33C4CA597B6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{95A49196-47DE-492C-ACAB-694926547D03}"/>
   </bookViews>
@@ -396,7 +396,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -406,6 +406,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFD3D3D3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,12 +449,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -779,12 +793,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7474037A-9BE1-4933-8F75-9508009AEEBF}">
   <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
+    <col min="3" max="3" width="65.44140625" customWidth="1"/>
     <col min="4" max="4" width="12.44140625" customWidth="1"/>
     <col min="5" max="5" width="10.77734375" customWidth="1"/>
     <col min="6" max="6" width="15.77734375" customWidth="1"/>
@@ -1165,7 +1181,7 @@
       <c r="L15" s="1"/>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1211,7 +1227,7 @@
       <c r="L17" s="1"/>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1259,7 +1275,7 @@
       <c r="L19" s="1"/>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1473,7 +1489,7 @@
       <c r="L28" s="1"/>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="2" t="s">

</xml_diff>